<commit_message>
Add price and correct suppliers
</commit_message>
<xml_diff>
--- a/NewData.xlsx
+++ b/NewData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anvarshagvaleev/Education/DataScience/University/BusinessAnalysis/exercise_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8377207-6172-AC48-B857-5491F5CC4C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFB3603-000A-7E4C-B292-E91A69711934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="347">
   <si>
     <t>id</t>
   </si>
@@ -1065,6 +1065,15 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>Пост_1</t>
+  </si>
+  <si>
+    <t>Пост_2</t>
+  </si>
+  <si>
+    <t>Пост_3</t>
   </si>
 </sst>
 </file>
@@ -12733,7 +12742,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12758,185 +12767,221 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f t="shared" ref="B2:B13" si="0">CONCATENATE("Поставщик_",A2)</f>
-        <v>Поставщик_1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>337</v>
+      <c r="B2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
+      <c r="B3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
+      <c r="B4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>115</v>
+      <c r="B5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>140</v>
+      <c r="B6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>143</v>
+      <c r="B7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>280</v>
+      <c r="B8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>338</v>
+      <c r="B9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>339</v>
+      <c r="B10" t="s">
+        <v>345</v>
+      </c>
+      <c r="C10" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>340</v>
+      <c r="B11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C11" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>341</v>
+      <c r="B12" t="s">
+        <v>345</v>
+      </c>
+      <c r="C12" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Поставщик_12</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>345</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" t="s">
+        <v>345</v>
+      </c>
+      <c r="C15" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>345</v>
+      </c>
+      <c r="C16" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>346</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>346</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>346</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>346</v>
+      </c>
+      <c r="C20" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>

</xml_diff>